<commit_message>
-m fifth session; task done
</commit_message>
<xml_diff>
--- a/20_VCD1IL_CODING.xlsx
+++ b/20_VCD1IL_CODING.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\va23007122\PycharmProjects\20_VCD1IL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF447D13-64D9-4494-BE4F-D99AD94B4D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B78CEC-5FDD-4278-B2B0-93497742BE53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11820" yWindow="2910" windowWidth="21600" windowHeight="11385" xr2:uid="{2A973080-C290-40B9-9BFC-264EA2B7152F}"/>
+    <workbookView xWindow="4215" yWindow="3135" windowWidth="21600" windowHeight="11385" xr2:uid="{2A973080-C290-40B9-9BFC-264EA2B7152F}"/>
   </bookViews>
   <sheets>
     <sheet name="Friction values" sheetId="1" r:id="rId1"/>
@@ -437,7 +437,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +537,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="2">
-        <v>0</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D7" s="2">
         <v>0.35</v>
@@ -551,7 +551,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="2">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="D8" s="2">
         <v>0.3</v>

</xml_diff>

<commit_message>
-m ninth session; task done - adjusted µ static values for gravel and sand by taking µ dynamic values
</commit_message>
<xml_diff>
--- a/20_VCD1IL_CODING.xlsx
+++ b/20_VCD1IL_CODING.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\va23007122\PycharmProjects\20_VCD1IL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B78CEC-5FDD-4278-B2B0-93497742BE53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FC00A7-1E23-41E3-A4AB-B6DBB73FCCBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4215" yWindow="3135" windowWidth="21600" windowHeight="11385" xr2:uid="{2A973080-C290-40B9-9BFC-264EA2B7152F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2A973080-C290-40B9-9BFC-264EA2B7152F}"/>
   </bookViews>
   <sheets>
     <sheet name="Friction values" sheetId="1" r:id="rId1"/>
@@ -437,7 +437,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +537,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="2">
-        <v>0.55000000000000004</v>
+        <v>0.35</v>
       </c>
       <c r="D7" s="2">
         <v>0.35</v>
@@ -551,7 +551,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="2">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="D8" s="2">
         <v>0.3</v>

</xml_diff>